<commit_message>
"Maven integration with jenkins"
</commit_message>
<xml_diff>
--- a/Excel/Controller.xlsx
+++ b/Excel/Controller.xlsx
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B4:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,7 +923,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>